<commit_message>
Framework modified - logging info added
</commit_message>
<xml_diff>
--- a/Data/Demo/Output/BatchA/Summary.xlsx
+++ b/Data/Demo/Output/BatchA/Summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8976"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7896"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
-    <t>Summary Created On 07/16/2018 13:54:50</t>
+    <t>Summary Created On 07/17/2018 11:59:07</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>